<commit_message>
Documentação final do projeto
</commit_message>
<xml_diff>
--- a/documentacao/Banco-de-Dados/Dicionário de dados.xlsx
+++ b/documentacao/Banco-de-Dados/Dicionário de dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\coold\documentacao\Banco-de-Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\coold\documentacao\Banco-de-Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -763,7 +763,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>